<commit_message>
Tidy up of units for SoilWater in teh discussion document
</commit_message>
<xml_diff>
--- a/SoilWater.xlsx
+++ b/SoilWater.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceTree\Proj_UnitsInApsimX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX_Working\Proj_UnitsInApsimX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="42705" windowHeight="13320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="42703" windowHeight="13327"/>
   </bookViews>
   <sheets>
     <sheet name="SoilWater" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -404,18 +404,9 @@
     <t>dd-mmm</t>
   </si>
   <si>
-    <t>Start date for switch to summer parameters for evaporation</t>
-  </si>
-  <si>
     <t>Stage 2 drying coefficient for summer (a.k.a. ConA)</t>
   </si>
   <si>
-    <t>Cummulative evaporation to reach the end of stage 1 soil water evaporation in summer (a.k.a. U)</t>
-  </si>
-  <si>
-    <t>Start date for switch to winter parameters for evaporation</t>
-  </si>
-  <si>
     <t>Cummulative evaporation to reach the end of stage 1 soil water evaporation in winter (a.k.a. U)</t>
   </si>
   <si>
@@ -425,12 +416,6 @@
     <t>query units</t>
   </si>
   <si>
-    <t>Change in soil water diffusivity per unit change in volumetric soil water content</t>
-  </si>
-  <si>
-    <t>change with theta?</t>
-  </si>
-  <si>
     <t>Runoff Curve Number (CN) for bare soil with average moisture</t>
   </si>
   <si>
@@ -467,12 +452,6 @@
     <t>Maximum bare ground soil albedo</t>
   </si>
   <si>
-    <t>Factor to convert 'A' to coefficient in Adam's type residue effect on Eos</t>
-  </si>
-  <si>
-    <t>Coefficient in cover Eos reduction equation</t>
-  </si>
-  <si>
     <t>Critical sw ratio in top layer below which stage 2 evaporation occurs</t>
   </si>
   <si>
@@ -485,150 +464,24 @@
     <t>Efficiency of moving solute with unsaturated flow</t>
   </si>
   <si>
-    <t>Efficiency of moving solute with flux (saturated flow)</t>
-  </si>
-  <si>
-    <t>Gradient due to hydraulic differentials</t>
-  </si>
-  <si>
-    <t>Specific bulk density</t>
-  </si>
-  <si>
-    <t>Hydrologically effective depth for runoff</t>
-  </si>
-  <si>
     <t>Names of all possible mobile solutes</t>
   </si>
   <si>
     <t>Names of all possible immobile solutes</t>
   </si>
   <si>
-    <t>Canopy factors for cover runoff effect</t>
-  </si>
-  <si>
-    <t>Heights for canopy factors</t>
-  </si>
-  <si>
-    <t>Default canopy factor in absence of height</t>
-  </si>
-  <si>
-    <t>Name of soil evaporation model being used</t>
-  </si>
-  <si>
-    <t>Effective potential evapotranspiration</t>
-  </si>
-  <si>
-    <t>Potential evaporation after modification for green cover &amp; residue weight</t>
-  </si>
-  <si>
-    <t>descr?</t>
-  </si>
-  <si>
-    <t>Actual evaporation</t>
-  </si>
-  <si>
-    <t>Time after 2nd-stage that soil evaporation begins (d)</t>
-  </si>
-  <si>
-    <t>New cn2 after modification for crop cover &amp; residue cover</t>
-  </si>
-  <si>
-    <t>Drainage rate from bottom layer</t>
-  </si>
-  <si>
     <t>kg N /ha</t>
   </si>
   <si>
-    <t>Amount of N leaching as NO3</t>
-  </si>
-  <si>
-    <t>Amount of N leaching as NH4</t>
-  </si>
-  <si>
-    <t>Amount of N leaching as urea</t>
-  </si>
-  <si>
     <t>mm /d</t>
   </si>
   <si>
-    <t>unit?</t>
-  </si>
-  <si>
-    <t>Infiltration depth into top layer</t>
-  </si>
-  <si>
-    <t>Runoff from top layer</t>
-  </si>
-  <si>
     <t>Evaporation from the surface of the pond</t>
   </si>
   <si>
     <t>Surface water ponding depth</t>
   </si>
   <si>
-    <t>Extractable Soil Water (sw - ll15) of each layer summed over the profile.</t>
-  </si>
-  <si>
-    <t>Layer that irrigation went into.</t>
-  </si>
-  <si>
-    <t>Drained upper limit soil water content for each soil layer</t>
-  </si>
-  <si>
-    <t>Soil water content for each soil layer</t>
-  </si>
-  <si>
-    <t>Saturated water content for each soil layer</t>
-  </si>
-  <si>
-    <t>15 bar lower limit of extractable soil water for each soil layer</t>
-  </si>
-  <si>
-    <t>Thickness or depth of soil layers</t>
-  </si>
-  <si>
-    <t>Saturation of each layer</t>
-  </si>
-  <si>
-    <t>Air dry soil water content for each soil layer</t>
-  </si>
-  <si>
-    <t>Depth of water moving from layer i+1 into layer i because of unsaturated flow</t>
-  </si>
-  <si>
-    <t>Initially, water moving downward into layer i (mm), then water moving downward out of layer i (saturated flow)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outflowing lateral water </t>
-  </si>
-  <si>
-    <t>Temperature below which eeq (equilibrium evaporation rate) decreases</t>
-  </si>
-  <si>
-    <t>Temperature above which eeq (equilibrium evaporation rate) increases</t>
-  </si>
-  <si>
-    <t>Flow of N as NO3</t>
-  </si>
-  <si>
-    <t>Flow of N as NH4</t>
-  </si>
-  <si>
-    <t>Flow of N as urea</t>
-  </si>
-  <si>
-    <t>Residue interception loss (mm)</t>
-  </si>
-  <si>
-    <t>Delta soil water</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>0-1 /d</t>
-  </si>
-  <si>
     <t>Mg soil /m3 soil volume</t>
   </si>
   <si>
@@ -650,14 +503,185 @@
     <t>mm water /d</t>
   </si>
   <si>
-    <t>Depth below the ground surface of the first saturated layer</t>
+    <t>Cummulative soil water evaporation to reach the end of stage 1 soil water evaporation in summer (a.k.a. U)</t>
+  </si>
+  <si>
+    <t>Start date for switch to winter parameters for soil water evaporation</t>
+  </si>
+  <si>
+    <t>Start date for switch to summer parameters for soil water evaporation</t>
+  </si>
+  <si>
+    <t>Effect of soil water storage (in mm) above the lower limit on soil water diffusivity</t>
+  </si>
+  <si>
+    <t>The constant part of the soil water diffusivity calculation</t>
+  </si>
+  <si>
+    <t>Air temperature below which the ratio between eo and eeq decreases</t>
+  </si>
+  <si>
+    <t>Air temperature above which the ratio between eo and eeq increases</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A constant in the calculation of the effect of surface residues on eo</t>
+  </si>
+  <si>
+    <t>A constant in the calculation of the effect of canopy cover on eo</t>
+  </si>
+  <si>
+    <t>Efficiency of moving solute with flux (flux is the SoilWater term for saturated flow)</t>
+  </si>
+  <si>
+    <t>Constant of very mysterious units used in the calculation of the effect of gravity on the distribution of water across soil layers</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>Soil dry bulk density</t>
+  </si>
+  <si>
+    <t>Array of heights to use as lookup (X) values in relationship between crop height and effect of canopy cover on runoff</t>
+  </si>
+  <si>
+    <t>Array of values to use in the lookup (Y) values in relationship between crop height and effect of canopy cover on runoff</t>
+  </si>
+  <si>
+    <t>Default canopy factor in absence of the canopy_fact lookup</t>
+  </si>
+  <si>
+    <t>Name of soil water evaporation model being used</t>
+  </si>
+  <si>
+    <t>Potential evapotranspiration of the whole soil-plant system</t>
+  </si>
+  <si>
+    <t>Potential evaporation of water from the soil (after accounting for the effects of cover and residues)</t>
+  </si>
+  <si>
+    <t>Actual (realised) soil water evaporation</t>
+  </si>
+  <si>
+    <t>Number of days since 2nd-stage that soil water evaporation began</t>
+  </si>
+  <si>
+    <t>Actual curve number (CN) after takign into account the effects of crop and residue cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drainage exiting the deepest soil layer </t>
+  </si>
+  <si>
+    <t>Amount of N leaching as NO3 from the deepest soil layer</t>
+  </si>
+  <si>
+    <t>Amount of N leaching as NH4 from the deepest soil layer</t>
+  </si>
+  <si>
+    <t>Amount of N leaching as urea  from the deepest soil layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount of infiltration into the soil </t>
+  </si>
+  <si>
+    <t>Amount of runoff</t>
+  </si>
+  <si>
+    <t>Depth below the soil surface of the first saturated layer</t>
+  </si>
+  <si>
+    <t>Extractable soil water (sw_dep - ll15-dep) of each layer summed over the profile.</t>
+  </si>
+  <si>
+    <t>Soil layer to which irrigation was applied - 0 is surface (normal) irrigation, 1+ is the soil layer</t>
+  </si>
+  <si>
+    <t>Thicknesses or depths of the soil layers</t>
+  </si>
+  <si>
+    <t>Saturated water content for each soil layer expressed as a depth of water</t>
+  </si>
+  <si>
+    <t>Drained upper limit for each soil layer expressed as a depth of water</t>
+  </si>
+  <si>
+    <t>Current soil water content for each soil layer expressed as a depth of water</t>
+  </si>
+  <si>
+    <t>15 bar lower limit of extractable soil water for each soil layer expressed as a depth of water</t>
+  </si>
+  <si>
+    <t>Air dry soil water content for each soil layer expressed as a depth of water</t>
+  </si>
+  <si>
+    <t>Saturated water content for each soil layer expressed as a volumetric water content</t>
+  </si>
+  <si>
+    <t>Drained upper limit for each soil layer expressed as a volumetric water content</t>
+  </si>
+  <si>
+    <t>Current soil water content for each soil layer expressed as a volumetric water content</t>
+  </si>
+  <si>
+    <t>15 bar lower limit of extractable soil water for each soil layer expressed as a volumetric water content</t>
+  </si>
+  <si>
+    <t>Air dry soil water content for each soil layer expressed as a volumetric water content</t>
+  </si>
+  <si>
+    <t>Depth of water moving upward (i.e. from layer i+1 into layer i) because of unsaturated flow, a -ve value means downward movement</t>
+  </si>
+  <si>
+    <t>Depth of water moving downward out of each soil layer due to gravity drainage (at water contents above DUL)</t>
+  </si>
+  <si>
+    <t>Amount of water moving laterally out of the profile</t>
+  </si>
+  <si>
+    <t>Amount of N leaching as NO3 from each soil layer</t>
+  </si>
+  <si>
+    <t>Amount of N leaching as NH4 from each soil layer</t>
+  </si>
+  <si>
+    <t>Amount of N leaching as urea from each soil layer</t>
+  </si>
+  <si>
+    <t>Change in soil water depth in each soil layer</t>
+  </si>
+  <si>
+    <t>Change in volumetric soil water content in each soil layer</t>
+  </si>
+  <si>
+    <t>Loss of precipitation due in interception of surface residues</t>
+  </si>
+  <si>
+    <t>is this ever anything other than ritchie?</t>
+  </si>
+  <si>
+    <t>Something mysterious to do with the calculation of runoff</t>
+  </si>
+  <si>
+    <t>does this change with theta?</t>
+  </si>
+  <si>
+    <t>Querys?</t>
+  </si>
+  <si>
+    <t>Proposed display of units</t>
+  </si>
+  <si>
+    <t>Proposed Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,19 +702,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -720,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -734,10 +758,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,95 +1045,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="86.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="J2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>1</v>
@@ -1117,22 +1117,24 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="J3" s="2" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>1</v>
@@ -1143,22 +1145,22 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="J4" s="2" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>1</v>
@@ -1169,24 +1171,22 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="J5" s="2" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>1</v>
@@ -1197,22 +1197,24 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="J6" s="2" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>1</v>
@@ -1223,127 +1225,125 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="J7" s="2" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="J8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="E9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="E10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" s="2" t="s">
+      <c r="E11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K11" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="J11" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>6</v>
@@ -1352,7 +1352,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>1</v>
@@ -1363,24 +1363,24 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="J12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>1</v>
@@ -1391,15 +1391,15 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="J13" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>6</v>
@@ -1408,7 +1408,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>1</v>
@@ -1422,21 +1422,21 @@
         <v>9</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>1</v>
@@ -1447,24 +1447,24 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="J15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="b">
         <v>1</v>
@@ -1475,24 +1475,24 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="J16" s="2" t="s">
-        <v>124</v>
+        <v>8</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="2" t="b">
         <v>1</v>
@@ -1503,21 +1503,25 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="J17" s="2" t="s">
-        <v>202</v>
+        <v>124</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="2" t="b">
         <v>1</v>
       </c>
@@ -1527,25 +1531,21 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="J18" s="2" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2" t="b">
         <v>1</v>
       </c>
@@ -1555,24 +1555,24 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="J19" s="2" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>1</v>
@@ -1583,24 +1583,24 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="J20" s="2" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E21" s="2" t="b">
         <v>1</v>
@@ -1611,23 +1611,25 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="J21" s="2" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E22" s="2" t="b">
         <v>1</v>
       </c>
@@ -1637,15 +1639,15 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="J22" s="2" t="s">
-        <v>63</v>
+        <v>149</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
@@ -1663,21 +1665,21 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="J23" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="b">
@@ -1689,15 +1691,15 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="J24" s="2" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
@@ -1718,18 +1720,18 @@
         <v>9</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="b">
@@ -1741,21 +1743,21 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="J26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="b">
@@ -1767,21 +1769,21 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="J27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="b">
@@ -1793,15 +1795,15 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="J28" s="2" t="s">
-        <v>202</v>
+        <v>9</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
@@ -1819,21 +1821,21 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="J29" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="b">
@@ -1845,15 +1847,15 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="J30" s="2" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>54</v>
@@ -1874,15 +1876,15 @@
         <v>9</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
@@ -1900,44 +1902,46 @@
         <v>9</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="J33" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="b">
@@ -1949,39 +1953,43 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="J34" s="2" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="K34" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="K35" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="J35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>56</v>
@@ -2000,19 +2008,17 @@
         <v>18</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="b">
         <v>1</v>
@@ -2023,21 +2029,21 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="J37" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="b">
@@ -2049,21 +2055,21 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="J38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="b">
@@ -2075,20 +2081,22 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="J39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K39" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="b">
         <v>1</v>
@@ -2098,40 +2106,42 @@
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-      <c r="J40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K40" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="J41" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>6</v>
@@ -2147,19 +2157,17 @@
         <v>0</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H42" s="4"/>
       <c r="J42" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>6</v>
@@ -2175,25 +2183,23 @@
         <v>0</v>
       </c>
       <c r="G43" s="4"/>
-      <c r="H43" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H43" s="4"/>
       <c r="J43" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="b">
@@ -2205,46 +2211,46 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="J44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="J45" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F45" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="b">
         <v>0</v>
@@ -2253,25 +2259,23 @@
         <v>0</v>
       </c>
       <c r="G46" s="4"/>
-      <c r="H46" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="H46" s="4"/>
       <c r="J46" s="2" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="b">
@@ -2283,15 +2287,15 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="J47" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>6</v>
@@ -2309,15 +2313,15 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="J48" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>6</v>
@@ -2335,21 +2339,21 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="J49" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="b">
@@ -2361,15 +2365,15 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="J50" s="2" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>6</v>
@@ -2387,15 +2391,15 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="J51" s="2" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>6</v>
@@ -2413,15 +2417,15 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="J52" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>6</v>
@@ -2439,15 +2443,15 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="J53" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>6</v>
@@ -2457,7 +2461,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" s="2" t="b">
         <v>0</v>
@@ -2465,15 +2469,15 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="J54" s="2" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>6</v>
@@ -2483,7 +2487,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="2" t="b">
         <v>0</v>
@@ -2491,20 +2495,22 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="J55" s="2" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="b">
         <v>0</v>
@@ -2514,21 +2520,21 @@
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
-      <c r="J56" s="2"/>
+      <c r="J56" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="K56" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="b">
         <v>0</v>
@@ -2539,15 +2545,15 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="J57" s="2" t="s">
-        <v>205</v>
+        <v>18</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>54</v>
@@ -2565,15 +2571,15 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="J58" s="2" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>54</v>
@@ -2591,15 +2597,15 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="J59" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>54</v>
@@ -2609,7 +2615,7 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" s="2" t="b">
         <v>0</v>
@@ -2617,15 +2623,15 @@
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="J60" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>54</v>
@@ -2635,7 +2641,7 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="2" t="b">
         <v>0</v>
@@ -2643,15 +2649,15 @@
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="J61" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>54</v>
@@ -2669,21 +2675,21 @@
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="J62" s="2" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="b">
@@ -2695,15 +2701,15 @@
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="J63" s="2" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>54</v>
@@ -2724,12 +2730,12 @@
         <v>9</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>54</v>
@@ -2739,7 +2745,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="2" t="b">
         <v>0</v>
@@ -2750,12 +2756,12 @@
         <v>9</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>54</v>
@@ -2765,7 +2771,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" s="2" t="b">
         <v>0</v>
@@ -2776,12 +2782,12 @@
         <v>9</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>54</v>
@@ -2802,18 +2808,18 @@
         <v>9</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="b">
@@ -2825,15 +2831,15 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="J68" s="2" t="s">
-        <v>202</v>
+        <v>9</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>54</v>
@@ -2851,15 +2857,15 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="J69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K69" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K69" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>54</v>
@@ -2877,21 +2883,21 @@
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="J70" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="K70" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="b">
@@ -2901,19 +2907,17 @@
         <v>0</v>
       </c>
       <c r="G71" s="4"/>
-      <c r="H71" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H71" s="4"/>
       <c r="J71" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>54</v>
@@ -2929,19 +2933,17 @@
         <v>0</v>
       </c>
       <c r="G72" s="4"/>
-      <c r="H72" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H72" s="4"/>
       <c r="J72" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>54</v>
@@ -2957,53 +2959,49 @@
         <v>0</v>
       </c>
       <c r="G73" s="4"/>
-      <c r="H73" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H73" s="4"/>
       <c r="J73" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G74" s="4"/>
-      <c r="H74" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H74" s="4"/>
       <c r="J74" s="2" t="s">
-        <v>202</v>
+        <v>148</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2" t="b">
@@ -3013,25 +3011,23 @@
         <v>0</v>
       </c>
       <c r="G75" s="4"/>
-      <c r="H75" s="4" t="s">
-        <v>165</v>
-      </c>
+      <c r="H75" s="4"/>
       <c r="J75" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2" t="b">
@@ -3043,20 +3039,22 @@
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="J76" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="K76" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2" t="b">
         <v>1</v>
@@ -3066,15 +3064,19 @@
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J77" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -3089,12 +3091,12 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -3109,12 +3111,12 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -3129,17 +3131,17 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" s="2" t="b">
         <v>0</v>
@@ -3148,6 +3150,26 @@
       <c r="H81" s="4"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
+    </row>
+    <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>